<commit_message>
some misc changes, including creating the template for the victors spreadsheets
</commit_message>
<xml_diff>
--- a/production/data/city_politics.xlsx
+++ b/production/data/city_politics.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="680" windowWidth="25360" windowHeight="15380" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="680" windowWidth="15520" windowHeight="15380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -382,8 +382,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -407,7 +409,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -415,6 +417,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -422,6 +425,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -768,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA937"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -15385,49 +15389,49 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>17</v>
+      <c r="A4" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -15440,22 +15444,26 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B7">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="4" t="s">
-        <v>52</v>
+      <c r="A8" t="s">
+        <v>18</v>
       </c>
       <c r="B8">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A1:B8">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>